<commit_message>
can read new excel format
</commit_message>
<xml_diff>
--- a/uploads/gantt.xlsx
+++ b/uploads/gantt.xlsx
@@ -143,10 +143,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="167" formatCode="0%"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -261,7 +262,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,6 +285,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -366,28 +371,28 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="34.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="1021" min="20" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="1021" min="20" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -420,8 +425,8 @@
       <c r="D2" s="5" t="n">
         <v>42581</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>50</v>
+      <c r="E2" s="6" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -437,8 +442,8 @@
       <c r="D3" s="5" t="n">
         <v>42583</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>75</v>
+      <c r="E3" s="6" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -522,8 +527,8 @@
       <c r="D8" s="5" t="n">
         <v>42591</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>85</v>
+      <c r="E8" s="6" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>